<commit_message>
Background changes 1st draft
Copied the moveleft into moveup and moveright into movedown. Then edit the moveup and movedown.
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wustyheals\Documents\UWI COURSE WORK\2021\Semester 2\Game Programming\A3\Game-Programming-Assignment-3---Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC0DE1-49C7-43DE-8A7C-CABA865A8A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF46E8-A0F2-49EF-91D8-73234041F5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Design Document</t>
   </si>
@@ -206,14 +206,17 @@
     <t>Backgrount Manager</t>
   </si>
   <si>
-    <t>currently at line 133</t>
+    <t>Things to check if errors occur</t>
+  </si>
+  <si>
+    <t>getHeightPixels from tilemap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +238,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -367,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -413,6 +421,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,10 +804,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6026EE-B549-4AFB-9AC6-0EC1FB9D075A}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +818,7 @@
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
@@ -815,19 +826,19 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -841,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>11</v>
       </c>
@@ -851,7 +862,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -859,7 +870,7 @@
       <c r="C6" s="11"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="6" t="s">
         <v>20</v>
@@ -867,7 +878,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="6" t="s">
         <v>21</v>
@@ -875,7 +886,7 @@
       <c r="C8" s="13"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
@@ -883,7 +894,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
@@ -891,7 +902,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="14"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
         <v>24</v>
@@ -902,7 +913,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="6" t="s">
         <v>25</v>
@@ -912,11 +923,8 @@
       <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>23</v>
@@ -927,7 +935,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -938,7 +946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="6" t="s">
         <v>22</v>
@@ -949,7 +957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -957,7 +965,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="5" t="s">
         <v>24</v>
@@ -965,23 +973,29 @@
       <c r="C17" s="12"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="6" t="s">
         <v>26</v>
@@ -989,7 +1003,7 @@
       <c r="C20" s="13"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>22</v>
@@ -997,13 +1011,13 @@
       <c r="C21" s="12"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="5"/>
       <c r="C22" s="11"/>
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>13</v>
       </c>
@@ -1011,7 +1025,7 @@
       <c r="C23" s="8"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="6" t="s">
         <v>28</v>
@@ -1019,7 +1033,7 @@
       <c r="C24" s="13"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>29</v>
@@ -1027,7 +1041,7 @@
       <c r="C25" s="12"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>30</v>
@@ -1035,7 +1049,7 @@
       <c r="C26" s="11"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="6" t="s">
         <v>31</v>
@@ -1043,7 +1057,7 @@
       <c r="C27" s="8"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="6" t="s">
         <v>22</v>
@@ -1051,7 +1065,7 @@
       <c r="C28" s="13"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>14</v>
       </c>
@@ -1059,7 +1073,7 @@
       <c r="C29" s="12"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>28</v>
@@ -1067,7 +1081,7 @@
       <c r="C30" s="11"/>
       <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="6" t="s">
         <v>29</v>
@@ -1075,7 +1089,7 @@
       <c r="C31" s="8"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="6" t="s">
         <v>30</v>
@@ -1339,19 +1353,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A52"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A1:D3"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Got the Background working
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wustyheals\Documents\UWI COURSE WORK\2021\Semester 2\Game Programming\A3\Game-Programming-Assignment-3---Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF46E8-A0F2-49EF-91D8-73234041F5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BE2FA8-D3F3-4059-836B-5A19A870AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8010" yWindow="1845" windowWidth="12480" windowHeight="6285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Design Document</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>getHeightPixels from tilemap</t>
+  </si>
+  <si>
+    <t>Note to self</t>
+  </si>
+  <si>
+    <t>week 6 fading bg</t>
   </si>
 </sst>
 </file>
@@ -392,6 +398,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -421,9 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,24 +724,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -752,7 +758,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -763,19 +769,19 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -784,7 +790,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -806,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6026EE-B549-4AFB-9AC6-0EC1FB9D075A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,24 +825,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -853,7 +859,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -863,7 +869,7 @@
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
@@ -871,7 +877,7 @@
       <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
@@ -879,7 +885,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
@@ -887,7 +893,7 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
@@ -895,7 +901,7 @@
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="5"/>
@@ -903,7 +909,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
@@ -914,7 +920,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
@@ -925,7 +931,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
@@ -936,7 +942,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
@@ -947,7 +953,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
@@ -958,7 +964,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="6"/>
@@ -966,7 +972,7 @@
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
@@ -974,7 +980,7 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
@@ -985,18 +991,18 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="10"/>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1010,7 @@
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1012,21 +1018,27 @@
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="5"/>
       <c r="C22" s="11"/>
       <c r="D22" s="14"/>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="10"/>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="6" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1046,7 @@
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="5" t="s">
         <v>29</v>
       </c>
@@ -1042,7 +1054,7 @@
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
@@ -1050,7 +1062,7 @@
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="6" t="s">
         <v>31</v>
       </c>
@@ -1058,7 +1070,7 @@
       <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="6" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1078,7 @@
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="5"/>
@@ -1074,7 +1086,7 @@
       <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="5" t="s">
         <v>28</v>
       </c>
@@ -1082,7 +1094,7 @@
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="6" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1102,7 @@
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="6" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1110,7 @@
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="5" t="s">
         <v>31</v>
       </c>
@@ -1106,7 +1118,7 @@
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="5" t="s">
         <v>22</v>
       </c>
@@ -1114,7 +1126,7 @@
       <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -1124,7 +1136,7 @@
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="6" t="s">
         <v>33</v>
       </c>
@@ -1132,7 +1144,7 @@
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="5" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1152,7 @@
       <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="5" t="s">
         <v>35</v>
       </c>
@@ -1148,7 +1160,7 @@
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="6" t="s">
         <v>36</v>
       </c>
@@ -1156,7 +1168,7 @@
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="6" t="s">
         <v>22</v>
       </c>
@@ -1164,7 +1176,7 @@
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="20" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="5"/>
@@ -1172,7 +1184,7 @@
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
@@ -1180,7 +1192,7 @@
       <c r="D42" s="14"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="6" t="s">
         <v>38</v>
       </c>
@@ -1188,7 +1200,7 @@
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="6" t="s">
         <v>39</v>
       </c>
@@ -1196,7 +1208,7 @@
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="5" t="s">
         <v>40</v>
       </c>
@@ -1204,7 +1216,7 @@
       <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="5" t="s">
         <v>22</v>
       </c>
@@ -1212,7 +1224,7 @@
       <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B47" s="6"/>
@@ -1220,7 +1232,7 @@
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="6" t="s">
         <v>41</v>
       </c>
@@ -1228,7 +1240,7 @@
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="5" t="s">
         <v>35</v>
       </c>
@@ -1236,7 +1248,7 @@
       <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="5" t="s">
         <v>31</v>
       </c>
@@ -1244,13 +1256,13 @@
       <c r="D50" s="14"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="6"/>
       <c r="C51" s="8"/>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="6" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1270,7 @@
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="5"/>
@@ -1266,7 +1278,7 @@
       <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="5" t="s">
         <v>37</v>
       </c>
@@ -1274,7 +1286,7 @@
       <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="6" t="s">
         <v>40</v>
       </c>
@@ -1282,7 +1294,7 @@
       <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="6" t="s">
         <v>22</v>
       </c>
@@ -1290,19 +1302,19 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="5"/>
       <c r="C57" s="12"/>
       <c r="D57" s="9"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="5"/>
       <c r="C58" s="11"/>
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -1314,7 +1326,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="6" t="s">
         <v>51</v>
       </c>
@@ -1322,7 +1334,7 @@
       <c r="D60" s="10"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="5" t="s">
         <v>35</v>
       </c>
@@ -1330,7 +1342,7 @@
       <c r="D61" s="9"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="5" t="s">
         <v>31</v>
       </c>
@@ -1338,13 +1350,13 @@
       <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+      <c r="A63" s="20"/>
       <c r="B63" s="6"/>
       <c r="C63" s="8"/>
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="6" t="s">
         <v>22</v>
       </c>
@@ -1353,17 +1365,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A52"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A1:D3"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1385,27 +1397,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
@@ -1413,23 +1425,23 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="15"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B11" t="s">
@@ -1437,22 +1449,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B17" t="s">
@@ -1460,19 +1472,19 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Map 2 and combat system Update 1
Added systems for testing map 2 and combat map as well as initial changes for map 2
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wustyheals\Documents\UWI COURSE WORK\2021\Semester 2\Game Programming\A3\Game-Programming-Assignment-3---Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BE2FA8-D3F3-4059-836B-5A19A870AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A297A26-842C-4F82-9AAD-B067CAB97864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="1845" windowWidth="12480" windowHeight="6285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>Design Document</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>week 6 fading bg</t>
+  </si>
+  <si>
+    <t>started implementing chap 2 and combat system</t>
+  </si>
+  <si>
+    <t>Refactor Player class to not use tilemap</t>
+  </si>
+  <si>
+    <t>reInstanciate in GameWindow</t>
+  </si>
+  <si>
+    <t>Player not moving to the right in map 2 because tilemap code is not working on that map</t>
   </si>
 </sst>
 </file>
@@ -812,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6026EE-B549-4AFB-9AC6-0EC1FB9D075A}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,6 +1072,9 @@
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="14"/>
+      <c r="F26" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
@@ -1076,6 +1091,9 @@
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="10"/>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
@@ -1084,6 +1102,9 @@
       <c r="B29" s="5"/>
       <c r="C29" s="12"/>
       <c r="D29" s="9"/>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
@@ -1092,6 +1113,9 @@
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="14"/>
+      <c r="F30" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
@@ -1133,7 +1157,9 @@
         <v>32</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
@@ -1331,7 +1357,9 @@
         <v>51</v>
       </c>
       <c r="C60" s="13"/>
-      <c r="D60" s="10"/>
+      <c r="D60" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
@@ -1365,17 +1393,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A52"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A1:D3"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>